<commit_message>
Salvando alterações novas | Agora fiz um script novo que usa uma base com os nomes das marcas para não ter que usar o dropdown | Fiz tbm um código que usa os códigos fipes para pesquisar
</commit_message>
<xml_diff>
--- a/Fipe_temp_motos.xlsx
+++ b/Fipe_temp_motos.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="65">
   <si>
     <t>MarcaSelecionada</t>
   </si>
@@ -43,6 +43,18 @@
     <t>AGRALE</t>
   </si>
   <si>
+    <t>BAJAJ</t>
+  </si>
+  <si>
+    <t>APRILIA</t>
+  </si>
+  <si>
+    <t>GARINNI</t>
+  </si>
+  <si>
+    <t>MOTORINO</t>
+  </si>
+  <si>
     <t>AME-110 MIX</t>
   </si>
   <si>
@@ -58,9 +70,90 @@
     <t>AME-150 TC/ SC</t>
   </si>
   <si>
+    <t>DOMINAR 160</t>
+  </si>
+  <si>
+    <t>LEONARDO 150cc</t>
+  </si>
+  <si>
+    <t>AME-LX 125/26</t>
+  </si>
+  <si>
+    <t>DAKAR 50</t>
+  </si>
+  <si>
+    <t>DOMINAR 250</t>
+  </si>
+  <si>
+    <t>PEGASO 650cc</t>
+  </si>
+  <si>
+    <t>DOMINAR 400</t>
+  </si>
+  <si>
+    <t>ELEFANT 16.5 125cc</t>
+  </si>
+  <si>
+    <t>CITY 50</t>
+  </si>
+  <si>
+    <t>ATV 50</t>
+  </si>
+  <si>
+    <t>GR08T4</t>
+  </si>
+  <si>
+    <t>Bacio 125cc</t>
+  </si>
+  <si>
+    <t>Zero KM</t>
+  </si>
+  <si>
+    <t>1999</t>
+  </si>
+  <si>
+    <t>2007</t>
+  </si>
+  <si>
+    <t>2009</t>
+  </si>
+  <si>
+    <t>1998</t>
+  </si>
+  <si>
+    <t>2006</t>
+  </si>
+  <si>
+    <t>1997</t>
+  </si>
+  <si>
+    <t>2001</t>
+  </si>
+  <si>
     <t>2008</t>
   </si>
   <si>
+    <t>2000</t>
+  </si>
+  <si>
+    <t>1990</t>
+  </si>
+  <si>
+    <t>2002</t>
+  </si>
+  <si>
+    <t>1993</t>
+  </si>
+  <si>
+    <t>1992</t>
+  </si>
+  <si>
+    <t>2014</t>
+  </si>
+  <si>
+    <t>2011</t>
+  </si>
+  <si>
     <t>855004-2</t>
   </si>
   <si>
@@ -76,7 +169,43 @@
     <t>855002-6</t>
   </si>
   <si>
-    <t xml:space="preserve"> 3063.00</t>
+    <t>837004-4</t>
+  </si>
+  <si>
+    <t>802003-5</t>
+  </si>
+  <si>
+    <t>855003-4</t>
+  </si>
+  <si>
+    <t>801005-6</t>
+  </si>
+  <si>
+    <t>837006-0</t>
+  </si>
+  <si>
+    <t>802005-1</t>
+  </si>
+  <si>
+    <t>837003-6</t>
+  </si>
+  <si>
+    <t>801007-2</t>
+  </si>
+  <si>
+    <t>801002-1</t>
+  </si>
+  <si>
+    <t>840014-8</t>
+  </si>
+  <si>
+    <t>847001-4</t>
+  </si>
+  <si>
+    <t>881008-7</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 6301.00</t>
   </si>
   <si>
     <t>julho de 2025</t>
@@ -437,7 +566,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -468,19 +597,19 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C2">
         <v>2009</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="E2">
         <v>2190</v>
       </c>
       <c r="F2" t="s">
-        <v>21</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -488,19 +617,19 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C3">
         <v>2002</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="E3">
         <v>3784</v>
       </c>
       <c r="F3" t="s">
-        <v>21</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -508,19 +637,19 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C4">
         <v>2008</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="E4">
         <v>1993</v>
       </c>
       <c r="F4" t="s">
-        <v>21</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -528,19 +657,19 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C5">
         <v>2009</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="E5">
         <v>10919</v>
       </c>
       <c r="F5" t="s">
-        <v>21</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -548,19 +677,19 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C6">
         <v>2007</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="E6">
         <v>1776</v>
       </c>
       <c r="F6" t="s">
-        <v>21</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -568,19 +697,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C7">
         <v>2006</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="E7">
         <v>1611</v>
       </c>
       <c r="F7" t="s">
-        <v>21</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -588,19 +717,19 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C8">
         <v>1993</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="E8">
         <v>1666</v>
       </c>
       <c r="F8" t="s">
-        <v>21</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -608,19 +737,19 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C9">
         <v>2006</v>
       </c>
       <c r="D9" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="E9">
         <v>2510</v>
       </c>
       <c r="F9" t="s">
-        <v>21</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -628,19 +757,19 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C10">
         <v>1992</v>
       </c>
       <c r="D10" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="E10">
         <v>1481</v>
       </c>
       <c r="F10" t="s">
-        <v>21</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -648,19 +777,759 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11">
+        <v>2008</v>
+      </c>
+      <c r="D11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11">
+        <v>3063</v>
+      </c>
+      <c r="F11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12">
+        <v>1991</v>
+      </c>
+      <c r="D12" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12">
+        <v>1365</v>
+      </c>
+      <c r="F12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13">
+        <v>17500</v>
+      </c>
+      <c r="F13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14">
+        <v>6527</v>
+      </c>
+      <c r="F14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15">
+        <v>2793</v>
+      </c>
+      <c r="F15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16">
+        <v>2437</v>
+      </c>
+      <c r="F16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17">
+        <v>5864</v>
+      </c>
+      <c r="F17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18">
+        <v>2510</v>
+      </c>
+      <c r="F18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19">
+        <v>1816</v>
+      </c>
+      <c r="F19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" t="s">
+        <v>54</v>
+      </c>
+      <c r="E20">
+        <v>1571</v>
+      </c>
+      <c r="F20" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" t="s">
+        <v>53</v>
+      </c>
+      <c r="E21">
+        <v>1685</v>
+      </c>
+      <c r="F21" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" t="s">
+        <v>55</v>
+      </c>
+      <c r="E22">
+        <v>22826</v>
+      </c>
+      <c r="F22" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" t="s">
+        <v>54</v>
+      </c>
+      <c r="E23">
+        <v>1476</v>
+      </c>
+      <c r="F23" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" t="s">
+        <v>56</v>
+      </c>
+      <c r="E24">
+        <v>14759</v>
+      </c>
+      <c r="F24" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" t="s">
+        <v>48</v>
+      </c>
+      <c r="E25">
+        <v>9686</v>
+      </c>
+      <c r="F25" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" t="s">
+        <v>56</v>
+      </c>
+      <c r="E26">
+        <v>12950</v>
+      </c>
+      <c r="F26" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" t="s">
+        <v>48</v>
+      </c>
+      <c r="E27">
+        <v>9047</v>
+      </c>
+      <c r="F27" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" t="s">
+        <v>57</v>
+      </c>
+      <c r="E28">
+        <v>25834</v>
+      </c>
+      <c r="F28" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29" t="s">
+        <v>40</v>
+      </c>
+      <c r="D29" t="s">
+        <v>58</v>
+      </c>
+      <c r="E29">
+        <v>1271</v>
+      </c>
+      <c r="F29" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" t="s">
+        <v>35</v>
+      </c>
+      <c r="D30" t="s">
+        <v>48</v>
+      </c>
+      <c r="E30">
+        <v>8041</v>
+      </c>
+      <c r="F30" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" t="s">
         <v>13</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C31" t="s">
+        <v>33</v>
+      </c>
+      <c r="D31" t="s">
+        <v>46</v>
+      </c>
+      <c r="E31">
+        <v>2190</v>
+      </c>
+      <c r="F31" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" t="s">
         <v>14</v>
       </c>
-      <c r="D11" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" t="s">
-        <v>21</v>
+      <c r="C32" t="s">
+        <v>41</v>
+      </c>
+      <c r="D32" t="s">
+        <v>47</v>
+      </c>
+      <c r="E32">
+        <v>3784</v>
+      </c>
+      <c r="F32" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" t="s">
+        <v>38</v>
+      </c>
+      <c r="D33" t="s">
+        <v>46</v>
+      </c>
+      <c r="E33">
+        <v>1993</v>
+      </c>
+      <c r="F33" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" t="s">
+        <v>33</v>
+      </c>
+      <c r="D34" t="s">
+        <v>48</v>
+      </c>
+      <c r="E34">
+        <v>10919</v>
+      </c>
+      <c r="F34" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35" t="s">
+        <v>32</v>
+      </c>
+      <c r="D35" t="s">
+        <v>46</v>
+      </c>
+      <c r="E35">
+        <v>1776</v>
+      </c>
+      <c r="F35" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36" t="s">
+        <v>16</v>
+      </c>
+      <c r="C36" t="s">
+        <v>42</v>
+      </c>
+      <c r="D36" t="s">
+        <v>49</v>
+      </c>
+      <c r="E36">
+        <v>1666</v>
+      </c>
+      <c r="F36" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37" t="s">
+        <v>35</v>
+      </c>
+      <c r="D37" t="s">
+        <v>46</v>
+      </c>
+      <c r="E37">
+        <v>1611</v>
+      </c>
+      <c r="F37" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38" t="s">
+        <v>16</v>
+      </c>
+      <c r="C38" t="s">
+        <v>43</v>
+      </c>
+      <c r="D38" t="s">
+        <v>49</v>
+      </c>
+      <c r="E38">
+        <v>1481</v>
+      </c>
+      <c r="F38" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B39" t="s">
+        <v>26</v>
+      </c>
+      <c r="C39" t="s">
+        <v>37</v>
+      </c>
+      <c r="D39" t="s">
+        <v>59</v>
+      </c>
+      <c r="E39">
+        <v>1563</v>
+      </c>
+      <c r="F39" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" t="s">
+        <v>8</v>
+      </c>
+      <c r="B40" t="s">
+        <v>26</v>
+      </c>
+      <c r="C40" t="s">
+        <v>39</v>
+      </c>
+      <c r="D40" t="s">
+        <v>59</v>
+      </c>
+      <c r="E40">
+        <v>1523</v>
+      </c>
+      <c r="F40" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" t="s">
+        <v>7</v>
+      </c>
+      <c r="B41" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41" t="s">
+        <v>37</v>
+      </c>
+      <c r="D41" t="s">
+        <v>47</v>
+      </c>
+      <c r="E41">
+        <v>3388</v>
+      </c>
+      <c r="F41" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" t="s">
+        <v>39</v>
+      </c>
+      <c r="D42" t="s">
+        <v>47</v>
+      </c>
+      <c r="E42">
+        <v>3241</v>
+      </c>
+      <c r="F42" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" t="s">
+        <v>8</v>
+      </c>
+      <c r="B43" t="s">
+        <v>26</v>
+      </c>
+      <c r="C43" t="s">
+        <v>31</v>
+      </c>
+      <c r="D43" t="s">
+        <v>59</v>
+      </c>
+      <c r="E43">
+        <v>1439</v>
+      </c>
+      <c r="F43" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44" t="s">
+        <v>27</v>
+      </c>
+      <c r="C44" t="s">
+        <v>39</v>
+      </c>
+      <c r="D44" t="s">
+        <v>60</v>
+      </c>
+      <c r="E44">
+        <v>2437</v>
+      </c>
+      <c r="F44" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" t="s">
+        <v>11</v>
+      </c>
+      <c r="B45" t="s">
+        <v>28</v>
+      </c>
+      <c r="C45" t="s">
+        <v>32</v>
+      </c>
+      <c r="D45" t="s">
+        <v>61</v>
+      </c>
+      <c r="E45">
+        <v>1968</v>
+      </c>
+      <c r="F45" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46" t="s">
+        <v>29</v>
+      </c>
+      <c r="C46" t="s">
+        <v>44</v>
+      </c>
+      <c r="D46" t="s">
+        <v>62</v>
+      </c>
+      <c r="E46">
+        <v>6593</v>
+      </c>
+      <c r="F46" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" t="s">
+        <v>11</v>
+      </c>
+      <c r="B47" t="s">
+        <v>28</v>
+      </c>
+      <c r="C47" t="s">
+        <v>35</v>
+      </c>
+      <c r="D47" t="s">
+        <v>61</v>
+      </c>
+      <c r="E47">
+        <v>1743</v>
+      </c>
+      <c r="F47" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" t="s">
+        <v>12</v>
+      </c>
+      <c r="B48" t="s">
+        <v>29</v>
+      </c>
+      <c r="C48" t="s">
+        <v>45</v>
+      </c>
+      <c r="D48" t="s">
+        <v>62</v>
+      </c>
+      <c r="E48" t="s">
+        <v>63</v>
+      </c>
+      <c r="F48" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>